<commit_message>
CS1. Market data updated.
</commit_message>
<xml_diff>
--- a/data/CS1/Market Data/CS1_market_data_2020.xlsx
+++ b/data/CS1/Market Data/CS1_market_data_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resource-planning-v2\data\CS1\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9D01A-A750-4518-862C-8294F23A2576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA2346C-7276-44DA-9AC1-F9BA1511AC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,150 +180,150 @@
       <sheetData sheetId="1">
         <row r="2">
           <cell r="B2">
-            <v>35.04</v>
+            <v>43.71</v>
           </cell>
           <cell r="C2">
-            <v>34.020000000000003</v>
+            <v>40.784999999999997</v>
           </cell>
           <cell r="D2">
-            <v>30</v>
+            <v>39.052499999999995</v>
           </cell>
           <cell r="E2">
-            <v>30.03</v>
+            <v>36.622500000000002</v>
           </cell>
           <cell r="F2">
-            <v>33.590000000000003</v>
+            <v>37.715000000000003</v>
           </cell>
           <cell r="G2">
-            <v>33.35</v>
+            <v>40.745000000000005</v>
           </cell>
           <cell r="H2">
-            <v>34.01</v>
+            <v>49.295000000000002</v>
           </cell>
           <cell r="I2">
-            <v>35.33</v>
+            <v>51.59</v>
           </cell>
           <cell r="J2">
-            <v>36.94</v>
+            <v>54.25</v>
           </cell>
           <cell r="K2">
-            <v>38.74</v>
+            <v>53.837499999999999</v>
           </cell>
           <cell r="L2">
-            <v>36.6</v>
+            <v>52.800000000000004</v>
           </cell>
           <cell r="M2">
-            <v>34.19</v>
+            <v>52.542499999999997</v>
           </cell>
           <cell r="N2">
-            <v>34</v>
+            <v>50.507499999999993</v>
           </cell>
           <cell r="O2">
-            <v>34</v>
+            <v>49.795000000000002</v>
           </cell>
           <cell r="P2">
-            <v>30</v>
+            <v>48.817500000000003</v>
           </cell>
           <cell r="Q2">
-            <v>28.8</v>
+            <v>48.914999999999999</v>
           </cell>
           <cell r="R2">
-            <v>29.9</v>
+            <v>49.67</v>
           </cell>
           <cell r="S2">
-            <v>38.25</v>
+            <v>52.125</v>
           </cell>
           <cell r="T2">
-            <v>39.950000000000003</v>
+            <v>54.620000000000005</v>
           </cell>
           <cell r="U2">
-            <v>41.45</v>
+            <v>55.040000000000006</v>
           </cell>
           <cell r="V2">
-            <v>44.83</v>
+            <v>53.769999999999996</v>
           </cell>
           <cell r="W2">
-            <v>44.82</v>
+            <v>50.392499999999998</v>
           </cell>
           <cell r="X2">
-            <v>40.9</v>
+            <v>45.482500000000002</v>
           </cell>
           <cell r="Y2">
-            <v>39.75</v>
+            <v>42.69</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>30.25</v>
+            <v>40.82</v>
           </cell>
           <cell r="C3">
-            <v>26.85</v>
+            <v>38.53</v>
           </cell>
           <cell r="D3">
-            <v>22.25</v>
+            <v>36.034999999999997</v>
           </cell>
           <cell r="E3">
-            <v>18.09</v>
+            <v>34.424999999999997</v>
           </cell>
           <cell r="F3">
-            <v>10</v>
+            <v>36.340000000000003</v>
           </cell>
           <cell r="G3">
-            <v>8</v>
+            <v>38.28</v>
           </cell>
           <cell r="H3">
-            <v>8.41</v>
+            <v>44.2</v>
           </cell>
           <cell r="I3">
-            <v>8.41</v>
+            <v>46.17</v>
           </cell>
           <cell r="J3">
-            <v>10.8</v>
+            <v>48.480000000000004</v>
           </cell>
           <cell r="K3">
-            <v>16.989999999999998</v>
+            <v>48.805</v>
           </cell>
           <cell r="L3">
-            <v>19.54</v>
+            <v>47.400000000000006</v>
           </cell>
           <cell r="M3">
-            <v>17.920000000000002</v>
+            <v>46.424999999999997</v>
           </cell>
           <cell r="N3">
-            <v>22.75</v>
+            <v>45.004999999999995</v>
           </cell>
           <cell r="O3">
-            <v>20</v>
+            <v>44.53</v>
           </cell>
           <cell r="P3">
-            <v>21.57</v>
+            <v>42.545000000000002</v>
           </cell>
           <cell r="Q3">
-            <v>19.399999999999999</v>
+            <v>42.21</v>
           </cell>
           <cell r="R3">
-            <v>23.8</v>
+            <v>43.08</v>
           </cell>
           <cell r="S3">
-            <v>29.3</v>
+            <v>47.5</v>
           </cell>
           <cell r="T3">
-            <v>35.270000000000003</v>
+            <v>49.730000000000004</v>
           </cell>
           <cell r="U3">
-            <v>41</v>
+            <v>50.510000000000005</v>
           </cell>
           <cell r="V3">
-            <v>43.02</v>
+            <v>50.79</v>
           </cell>
           <cell r="W3">
-            <v>43</v>
+            <v>48.534999999999997</v>
           </cell>
           <cell r="X3">
-            <v>41.37</v>
+            <v>43.954999999999998</v>
           </cell>
           <cell r="Y3">
-            <v>41.35</v>
+            <v>41.71</v>
           </cell>
         </row>
         <row r="4">
@@ -404,224 +404,224 @@
       <sheetData sheetId="2">
         <row r="2">
           <cell r="B2">
-            <v>2.68</v>
+            <v>25.342275000000001</v>
           </cell>
           <cell r="C2">
-            <v>3.23</v>
+            <v>24.594854999999999</v>
           </cell>
           <cell r="D2">
-            <v>7.6</v>
+            <v>27.759217499999998</v>
           </cell>
           <cell r="E2">
-            <v>4.3600000000000003</v>
+            <v>30.54975</v>
           </cell>
           <cell r="F2">
-            <v>4.41</v>
+            <v>32.125005000000002</v>
           </cell>
           <cell r="G2">
-            <v>5.98</v>
+            <v>29.361535</v>
           </cell>
           <cell r="H2">
-            <v>5.19</v>
+            <v>27.199200000000001</v>
           </cell>
           <cell r="I2">
-            <v>6.08</v>
+            <v>29.454137500000002</v>
           </cell>
           <cell r="J2">
-            <v>4.68</v>
+            <v>25.75685</v>
           </cell>
           <cell r="K2">
-            <v>4.45</v>
+            <v>23.352209999999999</v>
           </cell>
           <cell r="L2">
-            <v>6.58</v>
+            <v>22.9788</v>
           </cell>
           <cell r="M2">
-            <v>9.39</v>
+            <v>20.269462499999999</v>
           </cell>
           <cell r="N2">
-            <v>9.75</v>
+            <v>22.549799999999994</v>
           </cell>
           <cell r="O2">
-            <v>10.65</v>
+            <v>18.743400000000001</v>
           </cell>
           <cell r="P2">
-            <v>11.37</v>
+            <v>19.593999999999998</v>
           </cell>
           <cell r="Q2">
-            <v>11.01</v>
+            <v>16.172449999999998</v>
           </cell>
           <cell r="R2">
-            <v>4.37</v>
+            <v>12.758287500000002</v>
           </cell>
           <cell r="S2">
-            <v>5.17</v>
+            <v>14.871139999999999</v>
           </cell>
           <cell r="T2">
-            <v>6.09</v>
+            <v>10.08586</v>
           </cell>
           <cell r="U2">
-            <v>4.7699999999999996</v>
+            <v>8.7737250000000007</v>
           </cell>
           <cell r="V2">
-            <v>4.6399999999999997</v>
+            <v>9.8389550000000003</v>
           </cell>
           <cell r="W2">
-            <v>3.6</v>
+            <v>13.74175</v>
           </cell>
           <cell r="X2">
-            <v>4.26</v>
+            <v>16.117327500000002</v>
           </cell>
           <cell r="Y2">
-            <v>20.81</v>
+            <v>14.23521</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>27.12</v>
+            <v>20.34</v>
           </cell>
           <cell r="C3">
-            <v>28.52</v>
+            <v>21.39</v>
           </cell>
           <cell r="D3">
-            <v>39.049999999999997</v>
+            <v>29.287499999999998</v>
           </cell>
           <cell r="E3">
-            <v>44.27</v>
+            <v>33.202500000000001</v>
           </cell>
           <cell r="F3">
-            <v>48.18</v>
+            <v>36.134999999999998</v>
           </cell>
           <cell r="G3">
-            <v>47.89</v>
+            <v>35.917500000000004</v>
           </cell>
           <cell r="H3">
-            <v>47.56</v>
+            <v>35.67</v>
           </cell>
           <cell r="I3">
-            <v>49.85</v>
+            <v>37.387500000000003</v>
           </cell>
           <cell r="J3">
-            <v>46.4</v>
+            <v>34.799999999999997</v>
           </cell>
           <cell r="K3">
-            <v>40.1</v>
+            <v>30.075000000000003</v>
           </cell>
           <cell r="L3">
-            <v>41.24</v>
+            <v>30.93</v>
           </cell>
           <cell r="M3">
-            <v>33.729999999999997</v>
+            <v>25.297499999999999</v>
           </cell>
           <cell r="N3">
-            <v>38.44</v>
+            <v>28.83</v>
           </cell>
           <cell r="O3">
-            <v>28.68</v>
+            <v>21.509999999999998</v>
           </cell>
           <cell r="P3">
-            <v>30.2</v>
+            <v>22.65</v>
           </cell>
           <cell r="Q3">
-            <v>27.12</v>
+            <v>20.34</v>
           </cell>
           <cell r="R3">
-            <v>18.190000000000001</v>
+            <v>13.642500000000002</v>
           </cell>
           <cell r="S3">
-            <v>22.68</v>
+            <v>17.009999999999998</v>
           </cell>
           <cell r="T3">
-            <v>14.82</v>
+            <v>11.115</v>
           </cell>
           <cell r="U3">
-            <v>13</v>
+            <v>9.75</v>
           </cell>
           <cell r="V3">
-            <v>14.51</v>
+            <v>10.8825</v>
           </cell>
           <cell r="W3">
-            <v>17.04</v>
+            <v>12.78</v>
           </cell>
           <cell r="X3">
-            <v>18.21</v>
+            <v>13.657500000000001</v>
           </cell>
           <cell r="Y3">
-            <v>14</v>
+            <v>10.5</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>16.43</v>
+            <v>27.930999999999997</v>
           </cell>
           <cell r="C4">
-            <v>15.51</v>
+            <v>26.366999999999997</v>
           </cell>
           <cell r="D4">
-            <v>16.440000000000001</v>
+            <v>27.948</v>
           </cell>
           <cell r="E4">
-            <v>16.41</v>
+            <v>27.896999999999998</v>
           </cell>
           <cell r="F4">
-            <v>16.920000000000002</v>
+            <v>28.764000000000003</v>
           </cell>
           <cell r="G4">
-            <v>14.12</v>
+            <v>24.003999999999998</v>
           </cell>
           <cell r="H4">
-            <v>12.35</v>
+            <v>20.994999999999997</v>
           </cell>
           <cell r="I4">
-            <v>11.65</v>
+            <v>19.805</v>
           </cell>
           <cell r="J4">
-            <v>10.45</v>
+            <v>17.764999999999997</v>
           </cell>
           <cell r="K4">
-            <v>9.51</v>
+            <v>16.166999999999998</v>
           </cell>
           <cell r="L4">
-            <v>7.8</v>
+            <v>13.26</v>
           </cell>
           <cell r="M4">
-            <v>7.83</v>
+            <v>13.311</v>
           </cell>
           <cell r="N4">
-            <v>8.5500000000000007</v>
+            <v>14.535</v>
           </cell>
           <cell r="O4">
-            <v>8.5500000000000007</v>
+            <v>14.535</v>
           </cell>
           <cell r="P4">
-            <v>9.5</v>
+            <v>16.149999999999999</v>
           </cell>
           <cell r="Q4">
-            <v>7.45</v>
+            <v>12.664999999999999</v>
           </cell>
           <cell r="R4">
-            <v>6.27</v>
+            <v>10.658999999999999</v>
           </cell>
           <cell r="S4">
-            <v>6.98</v>
+            <v>11.866</v>
           </cell>
           <cell r="T4">
-            <v>5.21</v>
+            <v>8.8569999999999993</v>
           </cell>
           <cell r="U4">
-            <v>5.13</v>
+            <v>8.7210000000000001</v>
           </cell>
           <cell r="V4">
-            <v>5.41</v>
+            <v>9.1969999999999992</v>
           </cell>
           <cell r="W4">
-            <v>9.5</v>
+            <v>16.149999999999999</v>
           </cell>
           <cell r="X4">
-            <v>10.74</v>
+            <v>18.257999999999999</v>
           </cell>
           <cell r="Y4">
-            <v>10.74</v>
+            <v>18.257999999999999</v>
           </cell>
         </row>
       </sheetData>
@@ -858,13 +858,13 @@
             <v>24.97</v>
           </cell>
           <cell r="D2">
-            <v>0</v>
+            <v>24.97</v>
           </cell>
           <cell r="E2">
             <v>25.97</v>
           </cell>
           <cell r="F2">
-            <v>0</v>
+            <v>25.97</v>
           </cell>
           <cell r="G2">
             <v>24.97</v>
@@ -926,81 +926,81 @@
         </row>
         <row r="3">
           <cell r="B3">
-            <v>4.22</v>
+            <v>28.36</v>
           </cell>
           <cell r="C3">
-            <v>0</v>
+            <v>28.36</v>
           </cell>
           <cell r="D3">
-            <v>4.22</v>
+            <v>27.234999999999999</v>
           </cell>
           <cell r="E3">
-            <v>4.22</v>
+            <v>28.86</v>
           </cell>
           <cell r="F3">
-            <v>4.22</v>
+            <v>28.86</v>
           </cell>
           <cell r="G3">
-            <v>4.22</v>
+            <v>28.36</v>
           </cell>
           <cell r="H3">
-            <v>4.22</v>
+            <v>37.325000000000003</v>
           </cell>
           <cell r="I3">
-            <v>4.22</v>
+            <v>30.75</v>
           </cell>
           <cell r="J3">
-            <v>4.22</v>
+            <v>32.480000000000004</v>
           </cell>
           <cell r="K3">
-            <v>0</v>
+            <v>34.879999999999995</v>
           </cell>
           <cell r="L3">
-            <v>0</v>
+            <v>32.489999999999995</v>
           </cell>
           <cell r="M3">
-            <v>0</v>
+            <v>32.489999999999995</v>
           </cell>
           <cell r="N3">
-            <v>0</v>
+            <v>32.480000000000004</v>
           </cell>
           <cell r="O3">
-            <v>0</v>
+            <v>32.5</v>
           </cell>
           <cell r="P3">
-            <v>0</v>
+            <v>32.480000000000004</v>
           </cell>
           <cell r="Q3">
-            <v>0</v>
+            <v>32.480000000000004</v>
           </cell>
           <cell r="R3">
-            <v>0</v>
+            <v>34.885000000000005</v>
           </cell>
           <cell r="S3">
-            <v>5.8</v>
+            <v>36.875</v>
           </cell>
           <cell r="T3">
-            <v>5.9</v>
+            <v>36.875</v>
           </cell>
           <cell r="U3">
-            <v>5.9</v>
+            <v>36.875</v>
           </cell>
           <cell r="V3">
-            <v>6.1</v>
+            <v>36.875</v>
           </cell>
           <cell r="W3">
-            <v>5.9</v>
+            <v>35.370000000000005</v>
           </cell>
           <cell r="X3">
-            <v>5.6</v>
+            <v>30.75</v>
           </cell>
           <cell r="Y3">
-            <v>36.6</v>
+            <v>30.75</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0</v>
+            <v>31.75</v>
           </cell>
           <cell r="C4">
             <v>31.75</v>
@@ -1300,76 +1300,76 @@
       <sheetData sheetId="6">
         <row r="2">
           <cell r="B2">
-            <v>7.99</v>
+            <v>10.26</v>
           </cell>
           <cell r="C2">
-            <v>7.99</v>
+            <v>10.909500000000001</v>
           </cell>
           <cell r="D2">
-            <v>7.99</v>
+            <v>10.084849999999999</v>
           </cell>
           <cell r="E2">
-            <v>10.36</v>
+            <v>8.7750000000000004</v>
           </cell>
           <cell r="F2">
-            <v>9.69</v>
+            <v>7.9588000000000001</v>
           </cell>
           <cell r="G2">
-            <v>8.8800000000000008</v>
+            <v>6.3310499999999994</v>
           </cell>
           <cell r="H2">
-            <v>8.09</v>
+            <v>5.706900000000001</v>
           </cell>
           <cell r="I2">
-            <v>6.99</v>
+            <v>4.8929999999999998</v>
           </cell>
           <cell r="J2">
-            <v>2.69</v>
+            <v>4.0228999999999999</v>
           </cell>
           <cell r="K2">
-            <v>4.49</v>
+            <v>4.4879999999999995</v>
           </cell>
           <cell r="L2">
-            <v>6.49</v>
+            <v>4.2223500000000005</v>
           </cell>
           <cell r="M2">
-            <v>7.74</v>
+            <v>4.0441500000000001</v>
           </cell>
           <cell r="N2">
-            <v>7.65</v>
+            <v>3.6749999999999998</v>
           </cell>
           <cell r="O2">
-            <v>8.39</v>
+            <v>4.1912000000000003</v>
           </cell>
           <cell r="P2">
-            <v>9.49</v>
+            <v>4.4894500000000006</v>
           </cell>
           <cell r="Q2">
-            <v>8.32</v>
+            <v>3.9945499999999998</v>
           </cell>
           <cell r="R2">
-            <v>7.65</v>
+            <v>2.9760000000000004</v>
           </cell>
           <cell r="S2">
-            <v>6.37</v>
+            <v>2.5608</v>
           </cell>
           <cell r="T2">
-            <v>6.49</v>
+            <v>3.0141000000000004</v>
           </cell>
           <cell r="U2">
-            <v>6.49</v>
+            <v>2.2196999999999996</v>
           </cell>
           <cell r="V2">
-            <v>7.73</v>
+            <v>3.6414</v>
           </cell>
           <cell r="W2">
-            <v>8.56</v>
+            <v>6.7825499999999996</v>
           </cell>
           <cell r="X2">
-            <v>6.99</v>
+            <v>7.5711999999999993</v>
           </cell>
           <cell r="Y2">
-            <v>7.89</v>
+            <v>6.9015499999999994</v>
           </cell>
         </row>
         <row r="3">
@@ -1524,150 +1524,150 @@
       <sheetData sheetId="7">
         <row r="2">
           <cell r="B2">
-            <v>46.31</v>
+            <v>42.153333333333336</v>
           </cell>
           <cell r="C2">
-            <v>46.31</v>
+            <v>42.486666666666672</v>
           </cell>
           <cell r="D2">
-            <v>46.31</v>
+            <v>42.486666666666672</v>
           </cell>
           <cell r="E2">
-            <v>64.64</v>
+            <v>51.303333333333335</v>
           </cell>
           <cell r="F2">
-            <v>48.31</v>
+            <v>44.726666666666667</v>
           </cell>
           <cell r="G2">
-            <v>42</v>
+            <v>53.636666666666677</v>
           </cell>
           <cell r="H2">
-            <v>48.31</v>
+            <v>52.483333333333327</v>
           </cell>
           <cell r="I2">
-            <v>42</v>
+            <v>40.266666666666673</v>
           </cell>
           <cell r="J2">
-            <v>42</v>
+            <v>40.466666666666669</v>
           </cell>
           <cell r="K2">
-            <v>43</v>
+            <v>59.133333333333333</v>
           </cell>
           <cell r="L2">
-            <v>43</v>
+            <v>40.833333333333336</v>
           </cell>
           <cell r="M2">
-            <v>43</v>
+            <v>40.833333333333336</v>
           </cell>
           <cell r="N2">
-            <v>99</v>
+            <v>59.5</v>
           </cell>
           <cell r="O2">
-            <v>99</v>
+            <v>59.5</v>
           </cell>
           <cell r="P2">
-            <v>43</v>
+            <v>44.09</v>
           </cell>
           <cell r="Q2">
-            <v>43</v>
+            <v>40.800000000000004</v>
           </cell>
           <cell r="R2">
-            <v>43</v>
+            <v>40.800000000000004</v>
           </cell>
           <cell r="S2">
-            <v>43</v>
+            <v>41.06666666666667</v>
           </cell>
           <cell r="T2">
-            <v>43</v>
+            <v>40.866666666666667</v>
           </cell>
           <cell r="U2">
-            <v>43</v>
+            <v>44.09</v>
           </cell>
           <cell r="V2">
-            <v>43</v>
+            <v>40.6</v>
           </cell>
           <cell r="W2">
-            <v>48.31</v>
+            <v>45.860000000000007</v>
           </cell>
           <cell r="X2">
-            <v>35.4</v>
+            <v>37.6</v>
           </cell>
           <cell r="Y2">
-            <v>35.4</v>
+            <v>37.6</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>49.87</v>
+            <v>36.216666666666669</v>
           </cell>
           <cell r="C3">
-            <v>49.87</v>
+            <v>36.88333333333334</v>
           </cell>
           <cell r="D3">
-            <v>49.87</v>
+            <v>36.88333333333334</v>
           </cell>
           <cell r="E3">
-            <v>49.87</v>
+            <v>45.351666666666667</v>
           </cell>
           <cell r="F3">
-            <v>49.87</v>
+            <v>40.36333333333333</v>
           </cell>
           <cell r="G3">
-            <v>49.87</v>
+            <v>61.338333333333338</v>
           </cell>
           <cell r="H3">
+            <v>60.76166666666667</v>
+          </cell>
+          <cell r="I3">
+            <v>39.833333333333336</v>
+          </cell>
+          <cell r="J3">
+            <v>40.233333333333334</v>
+          </cell>
+          <cell r="K3">
+            <v>49.266666666666666</v>
+          </cell>
+          <cell r="L3">
+            <v>40.116666666666667</v>
+          </cell>
+          <cell r="M3">
+            <v>40.116666666666667</v>
+          </cell>
+          <cell r="N3">
+            <v>49.45</v>
+          </cell>
+          <cell r="O3">
+            <v>49.45</v>
+          </cell>
+          <cell r="P3">
+            <v>41.745000000000005</v>
+          </cell>
+          <cell r="Q3">
             <v>40.1</v>
           </cell>
-          <cell r="I3">
-            <v>39.4</v>
-          </cell>
-          <cell r="J3">
-            <v>39.4</v>
-          </cell>
-          <cell r="K3">
-            <v>95</v>
-          </cell>
-          <cell r="L3">
-            <v>40.1</v>
-          </cell>
-          <cell r="M3">
-            <v>40.1</v>
-          </cell>
-          <cell r="N3">
-            <v>40.1</v>
-          </cell>
-          <cell r="O3">
-            <v>40.1</v>
-          </cell>
-          <cell r="P3">
-            <v>49.87</v>
-          </cell>
-          <cell r="Q3">
+          <cell r="R3">
+            <v>40.400000000000006</v>
+          </cell>
+          <cell r="S3">
+            <v>40.63333333333334</v>
+          </cell>
+          <cell r="T3">
+            <v>40.533333333333331</v>
+          </cell>
+          <cell r="U3">
+            <v>41.745000000000005</v>
+          </cell>
+          <cell r="V3">
             <v>40</v>
           </cell>
-          <cell r="R3">
-            <v>39.4</v>
-          </cell>
-          <cell r="S3">
-            <v>40</v>
-          </cell>
-          <cell r="T3">
-            <v>39.4</v>
-          </cell>
-          <cell r="U3">
-            <v>49.87</v>
-          </cell>
-          <cell r="V3">
-            <v>39.4</v>
-          </cell>
           <cell r="W3">
-            <v>49.87</v>
+            <v>42.63</v>
           </cell>
           <cell r="X3">
-            <v>37.4</v>
+            <v>38.799999999999997</v>
           </cell>
           <cell r="Y3">
-            <v>37.4</v>
+            <v>38.799999999999997</v>
           </cell>
         </row>
         <row r="4">
@@ -1822,150 +1822,150 @@
         </row>
         <row r="3">
           <cell r="B3">
-            <v>39.4</v>
+            <v>27.917499999999997</v>
           </cell>
           <cell r="C3">
-            <v>39.4</v>
+            <v>27.917499999999997</v>
           </cell>
           <cell r="D3">
-            <v>39.4</v>
+            <v>27.917499999999997</v>
           </cell>
           <cell r="E3">
-            <v>39.4</v>
+            <v>27.917499999999997</v>
           </cell>
           <cell r="F3">
-            <v>39.4</v>
+            <v>31.63</v>
           </cell>
           <cell r="G3">
-            <v>7.06</v>
+            <v>23.537500000000001</v>
           </cell>
           <cell r="H3">
-            <v>29.97</v>
+            <v>29.28</v>
           </cell>
           <cell r="I3">
-            <v>20.55</v>
+            <v>26.9175</v>
           </cell>
           <cell r="J3">
-            <v>20.55</v>
+            <v>26.9175</v>
           </cell>
           <cell r="K3">
-            <v>36.65</v>
+            <v>30.950000000000003</v>
           </cell>
           <cell r="L3">
-            <v>36.65</v>
+            <v>33.162500000000001</v>
           </cell>
           <cell r="M3">
-            <v>36.65</v>
+            <v>30.935000000000002</v>
           </cell>
           <cell r="N3">
-            <v>29.97</v>
+            <v>29.265000000000001</v>
           </cell>
           <cell r="O3">
-            <v>29.97</v>
+            <v>29.265000000000001</v>
           </cell>
           <cell r="P3">
-            <v>29.97</v>
+            <v>31.4925</v>
           </cell>
           <cell r="Q3">
-            <v>36.65</v>
+            <v>30.92</v>
           </cell>
           <cell r="R3">
-            <v>36.65</v>
+            <v>33.162500000000001</v>
           </cell>
           <cell r="S3">
-            <v>36.65</v>
+            <v>30.92</v>
           </cell>
           <cell r="T3">
-            <v>36.65</v>
+            <v>30.92</v>
           </cell>
           <cell r="U3">
-            <v>36.65</v>
+            <v>30.92</v>
           </cell>
           <cell r="V3">
-            <v>36.65</v>
+            <v>30.92</v>
           </cell>
           <cell r="W3">
-            <v>29.97</v>
+            <v>29.25</v>
           </cell>
           <cell r="X3">
-            <v>26.19</v>
+            <v>28.305</v>
           </cell>
           <cell r="Y3">
-            <v>26.19</v>
+            <v>27.532499999999999</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>2.2200000000000002</v>
+            <v>31.744999999999997</v>
           </cell>
           <cell r="C4">
-            <v>2.2000000000000002</v>
+            <v>31.744999999999997</v>
           </cell>
           <cell r="D4">
-            <v>2.2200000000000002</v>
+            <v>31.744999999999997</v>
           </cell>
           <cell r="E4">
-            <v>2.2200000000000002</v>
+            <v>31.744999999999997</v>
           </cell>
           <cell r="F4">
-            <v>37.51</v>
+            <v>34.22</v>
           </cell>
           <cell r="G4">
-            <v>37.520000000000003</v>
+            <v>18.045000000000002</v>
           </cell>
           <cell r="H4">
-            <v>37.520000000000003</v>
+            <v>29.509999999999998</v>
           </cell>
           <cell r="I4">
-            <v>20.02</v>
+            <v>24.795000000000002</v>
           </cell>
           <cell r="J4">
-            <v>26</v>
+            <v>24.795000000000002</v>
           </cell>
           <cell r="K4">
-            <v>37.51</v>
+            <v>32.85</v>
           </cell>
           <cell r="L4">
-            <v>37.51</v>
+            <v>34.325000000000003</v>
           </cell>
           <cell r="M4">
-            <v>37.9</v>
+            <v>32.840000000000003</v>
           </cell>
           <cell r="N4">
-            <v>37.9</v>
+            <v>29.5</v>
           </cell>
           <cell r="O4">
-            <v>37.9</v>
+            <v>29.5</v>
           </cell>
           <cell r="P4">
-            <v>37.51</v>
+            <v>30.984999999999999</v>
           </cell>
           <cell r="Q4">
-            <v>37.51</v>
+            <v>32.83</v>
           </cell>
           <cell r="R4">
-            <v>25.67</v>
+            <v>34.325000000000003</v>
           </cell>
           <cell r="S4">
-            <v>37.51</v>
+            <v>32.83</v>
           </cell>
           <cell r="T4">
-            <v>37.51</v>
+            <v>32.83</v>
           </cell>
           <cell r="U4">
-            <v>37.51</v>
+            <v>32.83</v>
           </cell>
           <cell r="V4">
-            <v>37.51</v>
+            <v>32.83</v>
           </cell>
           <cell r="W4">
-            <v>37.51</v>
+            <v>29.490000000000002</v>
           </cell>
           <cell r="X4">
-            <v>30.19</v>
+            <v>27.6</v>
           </cell>
           <cell r="Y4">
-            <v>30.19</v>
+            <v>27.085000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -2240,7 +2240,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,99 +2422,99 @@
       </c>
       <c r="B2" s="2">
         <f>'[1]Energy, Winter'!B2*Scenarios!$B$6</f>
-        <v>35.04</v>
+        <v>43.71</v>
       </c>
       <c r="C2" s="2">
         <f>'[1]Energy, Winter'!C2*Scenarios!$B$6</f>
-        <v>34.020000000000003</v>
+        <v>40.784999999999997</v>
       </c>
       <c r="D2" s="2">
         <f>'[1]Energy, Winter'!D2*Scenarios!$B$6</f>
-        <v>30</v>
+        <v>39.052499999999995</v>
       </c>
       <c r="E2" s="2">
         <f>'[1]Energy, Winter'!E2*Scenarios!$B$6</f>
-        <v>30.03</v>
+        <v>36.622500000000002</v>
       </c>
       <c r="F2" s="2">
         <f>'[1]Energy, Winter'!F2*Scenarios!$B$6</f>
-        <v>33.590000000000003</v>
+        <v>37.715000000000003</v>
       </c>
       <c r="G2" s="2">
         <f>'[1]Energy, Winter'!G2*Scenarios!$B$6</f>
-        <v>33.35</v>
+        <v>40.745000000000005</v>
       </c>
       <c r="H2" s="2">
         <f>'[1]Energy, Winter'!H2*Scenarios!$B$6</f>
-        <v>34.01</v>
+        <v>49.295000000000002</v>
       </c>
       <c r="I2" s="2">
         <f>'[1]Energy, Winter'!I2*Scenarios!$B$6</f>
-        <v>35.33</v>
+        <v>51.59</v>
       </c>
       <c r="J2" s="2">
         <f>'[1]Energy, Winter'!J2*Scenarios!$B$6</f>
-        <v>36.94</v>
+        <v>54.25</v>
       </c>
       <c r="K2" s="2">
         <f>'[1]Energy, Winter'!K2*Scenarios!$B$6</f>
-        <v>38.74</v>
+        <v>53.837499999999999</v>
       </c>
       <c r="L2" s="2">
         <f>'[1]Energy, Winter'!L2*Scenarios!$B$6</f>
-        <v>36.6</v>
+        <v>52.800000000000004</v>
       </c>
       <c r="M2" s="2">
         <f>'[1]Energy, Winter'!M2*Scenarios!$B$6</f>
-        <v>34.19</v>
+        <v>52.542499999999997</v>
       </c>
       <c r="N2" s="2">
         <f>'[1]Energy, Winter'!N2*Scenarios!$B$6</f>
-        <v>34</v>
+        <v>50.507499999999993</v>
       </c>
       <c r="O2" s="2">
         <f>'[1]Energy, Winter'!O2*Scenarios!$B$6</f>
-        <v>34</v>
+        <v>49.795000000000002</v>
       </c>
       <c r="P2" s="2">
         <f>'[1]Energy, Winter'!P2*Scenarios!$B$6</f>
-        <v>30</v>
+        <v>48.817500000000003</v>
       </c>
       <c r="Q2" s="2">
         <f>'[1]Energy, Winter'!Q2*Scenarios!$B$6</f>
-        <v>28.8</v>
+        <v>48.914999999999999</v>
       </c>
       <c r="R2" s="2">
         <f>'[1]Energy, Winter'!R2*Scenarios!$B$6</f>
-        <v>29.9</v>
+        <v>49.67</v>
       </c>
       <c r="S2" s="2">
         <f>'[1]Energy, Winter'!S2*Scenarios!$B$6</f>
-        <v>38.25</v>
+        <v>52.125</v>
       </c>
       <c r="T2" s="2">
         <f>'[1]Energy, Winter'!T2*Scenarios!$B$6</f>
-        <v>39.950000000000003</v>
+        <v>54.620000000000005</v>
       </c>
       <c r="U2" s="2">
         <f>'[1]Energy, Winter'!U2*Scenarios!$B$6</f>
-        <v>41.45</v>
+        <v>55.040000000000006</v>
       </c>
       <c r="V2" s="2">
         <f>'[1]Energy, Winter'!V2*Scenarios!$B$6</f>
-        <v>44.83</v>
+        <v>53.769999999999996</v>
       </c>
       <c r="W2" s="2">
         <f>'[1]Energy, Winter'!W2*Scenarios!$B$6</f>
-        <v>44.82</v>
+        <v>50.392499999999998</v>
       </c>
       <c r="X2" s="2">
         <f>'[1]Energy, Winter'!X2*Scenarios!$B$6</f>
-        <v>40.9</v>
+        <v>45.482500000000002</v>
       </c>
       <c r="Y2" s="2">
         <f>'[1]Energy, Winter'!Y2*Scenarios!$B$6</f>
-        <v>39.75</v>
+        <v>42.69</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2523,99 +2523,99 @@
       </c>
       <c r="B3" s="2">
         <f>'[1]Energy, Winter'!B3*Scenarios!$B$6</f>
-        <v>30.25</v>
+        <v>40.82</v>
       </c>
       <c r="C3" s="2">
         <f>'[1]Energy, Winter'!C3*Scenarios!$B$6</f>
-        <v>26.85</v>
+        <v>38.53</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]Energy, Winter'!D3*Scenarios!$B$6</f>
-        <v>22.25</v>
+        <v>36.034999999999997</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]Energy, Winter'!E3*Scenarios!$B$6</f>
-        <v>18.09</v>
+        <v>34.424999999999997</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]Energy, Winter'!F3*Scenarios!$B$6</f>
-        <v>10</v>
+        <v>36.340000000000003</v>
       </c>
       <c r="G3" s="2">
         <f>'[1]Energy, Winter'!G3*Scenarios!$B$6</f>
-        <v>8</v>
+        <v>38.28</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]Energy, Winter'!H3*Scenarios!$B$6</f>
-        <v>8.41</v>
+        <v>44.2</v>
       </c>
       <c r="I3" s="2">
         <f>'[1]Energy, Winter'!I3*Scenarios!$B$6</f>
-        <v>8.41</v>
+        <v>46.17</v>
       </c>
       <c r="J3" s="2">
         <f>'[1]Energy, Winter'!J3*Scenarios!$B$6</f>
-        <v>10.8</v>
+        <v>48.480000000000004</v>
       </c>
       <c r="K3" s="2">
         <f>'[1]Energy, Winter'!K3*Scenarios!$B$6</f>
-        <v>16.989999999999998</v>
+        <v>48.805</v>
       </c>
       <c r="L3" s="2">
         <f>'[1]Energy, Winter'!L3*Scenarios!$B$6</f>
-        <v>19.54</v>
+        <v>47.400000000000006</v>
       </c>
       <c r="M3" s="2">
         <f>'[1]Energy, Winter'!M3*Scenarios!$B$6</f>
-        <v>17.920000000000002</v>
+        <v>46.424999999999997</v>
       </c>
       <c r="N3" s="2">
         <f>'[1]Energy, Winter'!N3*Scenarios!$B$6</f>
-        <v>22.75</v>
+        <v>45.004999999999995</v>
       </c>
       <c r="O3" s="2">
         <f>'[1]Energy, Winter'!O3*Scenarios!$B$6</f>
-        <v>20</v>
+        <v>44.53</v>
       </c>
       <c r="P3" s="2">
         <f>'[1]Energy, Winter'!P3*Scenarios!$B$6</f>
-        <v>21.57</v>
+        <v>42.545000000000002</v>
       </c>
       <c r="Q3" s="2">
         <f>'[1]Energy, Winter'!Q3*Scenarios!$B$6</f>
-        <v>19.399999999999999</v>
+        <v>42.21</v>
       </c>
       <c r="R3" s="2">
         <f>'[1]Energy, Winter'!R3*Scenarios!$B$6</f>
-        <v>23.8</v>
+        <v>43.08</v>
       </c>
       <c r="S3" s="2">
         <f>'[1]Energy, Winter'!S3*Scenarios!$B$6</f>
-        <v>29.3</v>
+        <v>47.5</v>
       </c>
       <c r="T3" s="2">
         <f>'[1]Energy, Winter'!T3*Scenarios!$B$6</f>
-        <v>35.270000000000003</v>
+        <v>49.730000000000004</v>
       </c>
       <c r="U3" s="2">
         <f>'[1]Energy, Winter'!U3*Scenarios!$B$6</f>
-        <v>41</v>
+        <v>50.510000000000005</v>
       </c>
       <c r="V3" s="2">
         <f>'[1]Energy, Winter'!V3*Scenarios!$B$6</f>
-        <v>43.02</v>
+        <v>50.79</v>
       </c>
       <c r="W3" s="2">
         <f>'[1]Energy, Winter'!W3*Scenarios!$B$6</f>
-        <v>43</v>
+        <v>48.534999999999997</v>
       </c>
       <c r="X3" s="2">
         <f>'[1]Energy, Winter'!X3*Scenarios!$B$6</f>
-        <v>41.37</v>
+        <v>43.954999999999998</v>
       </c>
       <c r="Y3" s="2">
         <f>'[1]Energy, Winter'!Y3*Scenarios!$B$6</f>
-        <v>41.35</v>
+        <v>41.71</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2870,99 +2870,99 @@
       </c>
       <c r="B2" s="2">
         <f>'[1]Secondary Reserve, Winter'!B2*Scenarios!$B$7</f>
-        <v>2.68</v>
+        <v>25.342275000000001</v>
       </c>
       <c r="C2" s="2">
         <f>'[1]Secondary Reserve, Winter'!C2*Scenarios!$B$7</f>
-        <v>3.23</v>
+        <v>24.594854999999999</v>
       </c>
       <c r="D2" s="2">
         <f>'[1]Secondary Reserve, Winter'!D2*Scenarios!$B$7</f>
-        <v>7.6</v>
+        <v>27.759217499999998</v>
       </c>
       <c r="E2" s="2">
         <f>'[1]Secondary Reserve, Winter'!E2*Scenarios!$B$7</f>
-        <v>4.3600000000000003</v>
+        <v>30.54975</v>
       </c>
       <c r="F2" s="2">
         <f>'[1]Secondary Reserve, Winter'!F2*Scenarios!$B$7</f>
-        <v>4.41</v>
+        <v>32.125005000000002</v>
       </c>
       <c r="G2" s="2">
         <f>'[1]Secondary Reserve, Winter'!G2*Scenarios!$B$7</f>
-        <v>5.98</v>
+        <v>29.361535</v>
       </c>
       <c r="H2" s="2">
         <f>'[1]Secondary Reserve, Winter'!H2*Scenarios!$B$7</f>
-        <v>5.19</v>
+        <v>27.199200000000001</v>
       </c>
       <c r="I2" s="2">
         <f>'[1]Secondary Reserve, Winter'!I2*Scenarios!$B$7</f>
-        <v>6.08</v>
+        <v>29.454137500000002</v>
       </c>
       <c r="J2" s="2">
         <f>'[1]Secondary Reserve, Winter'!J2*Scenarios!$B$7</f>
-        <v>4.68</v>
+        <v>25.75685</v>
       </c>
       <c r="K2" s="2">
         <f>'[1]Secondary Reserve, Winter'!K2*Scenarios!$B$7</f>
-        <v>4.45</v>
+        <v>23.352209999999999</v>
       </c>
       <c r="L2" s="2">
         <f>'[1]Secondary Reserve, Winter'!L2*Scenarios!$B$7</f>
-        <v>6.58</v>
+        <v>22.9788</v>
       </c>
       <c r="M2" s="2">
         <f>'[1]Secondary Reserve, Winter'!M2*Scenarios!$B$7</f>
-        <v>9.39</v>
+        <v>20.269462499999999</v>
       </c>
       <c r="N2" s="2">
         <f>'[1]Secondary Reserve, Winter'!N2*Scenarios!$B$7</f>
-        <v>9.75</v>
+        <v>22.549799999999994</v>
       </c>
       <c r="O2" s="2">
         <f>'[1]Secondary Reserve, Winter'!O2*Scenarios!$B$7</f>
-        <v>10.65</v>
+        <v>18.743400000000001</v>
       </c>
       <c r="P2" s="2">
         <f>'[1]Secondary Reserve, Winter'!P2*Scenarios!$B$7</f>
-        <v>11.37</v>
+        <v>19.593999999999998</v>
       </c>
       <c r="Q2" s="2">
         <f>'[1]Secondary Reserve, Winter'!Q2*Scenarios!$B$7</f>
-        <v>11.01</v>
+        <v>16.172449999999998</v>
       </c>
       <c r="R2" s="2">
         <f>'[1]Secondary Reserve, Winter'!R2*Scenarios!$B$7</f>
-        <v>4.37</v>
+        <v>12.758287500000002</v>
       </c>
       <c r="S2" s="2">
         <f>'[1]Secondary Reserve, Winter'!S2*Scenarios!$B$7</f>
-        <v>5.17</v>
+        <v>14.871139999999999</v>
       </c>
       <c r="T2" s="2">
         <f>'[1]Secondary Reserve, Winter'!T2*Scenarios!$B$7</f>
-        <v>6.09</v>
+        <v>10.08586</v>
       </c>
       <c r="U2" s="2">
         <f>'[1]Secondary Reserve, Winter'!U2*Scenarios!$B$7</f>
-        <v>4.7699999999999996</v>
+        <v>8.7737250000000007</v>
       </c>
       <c r="V2" s="2">
         <f>'[1]Secondary Reserve, Winter'!V2*Scenarios!$B$7</f>
-        <v>4.6399999999999997</v>
+        <v>9.8389550000000003</v>
       </c>
       <c r="W2" s="2">
         <f>'[1]Secondary Reserve, Winter'!W2*Scenarios!$B$7</f>
-        <v>3.6</v>
+        <v>13.74175</v>
       </c>
       <c r="X2" s="2">
         <f>'[1]Secondary Reserve, Winter'!X2*Scenarios!$B$7</f>
-        <v>4.26</v>
+        <v>16.117327500000002</v>
       </c>
       <c r="Y2" s="2">
         <f>'[1]Secondary Reserve, Winter'!Y2*Scenarios!$B$7</f>
-        <v>20.81</v>
+        <v>14.23521</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2971,99 +2971,99 @@
       </c>
       <c r="B3" s="2">
         <f>'[1]Secondary Reserve, Winter'!B3*Scenarios!$B$7</f>
-        <v>27.12</v>
+        <v>20.34</v>
       </c>
       <c r="C3" s="2">
         <f>'[1]Secondary Reserve, Winter'!C3*Scenarios!$B$7</f>
-        <v>28.52</v>
+        <v>21.39</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]Secondary Reserve, Winter'!D3*Scenarios!$B$7</f>
-        <v>39.049999999999997</v>
+        <v>29.287499999999998</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]Secondary Reserve, Winter'!E3*Scenarios!$B$7</f>
-        <v>44.27</v>
+        <v>33.202500000000001</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]Secondary Reserve, Winter'!F3*Scenarios!$B$7</f>
-        <v>48.18</v>
+        <v>36.134999999999998</v>
       </c>
       <c r="G3" s="2">
         <f>'[1]Secondary Reserve, Winter'!G3*Scenarios!$B$7</f>
-        <v>47.89</v>
+        <v>35.917500000000004</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]Secondary Reserve, Winter'!H3*Scenarios!$B$7</f>
-        <v>47.56</v>
+        <v>35.67</v>
       </c>
       <c r="I3" s="2">
         <f>'[1]Secondary Reserve, Winter'!I3*Scenarios!$B$7</f>
-        <v>49.85</v>
+        <v>37.387500000000003</v>
       </c>
       <c r="J3" s="2">
         <f>'[1]Secondary Reserve, Winter'!J3*Scenarios!$B$7</f>
-        <v>46.4</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="K3" s="2">
         <f>'[1]Secondary Reserve, Winter'!K3*Scenarios!$B$7</f>
-        <v>40.1</v>
+        <v>30.075000000000003</v>
       </c>
       <c r="L3" s="2">
         <f>'[1]Secondary Reserve, Winter'!L3*Scenarios!$B$7</f>
-        <v>41.24</v>
+        <v>30.93</v>
       </c>
       <c r="M3" s="2">
         <f>'[1]Secondary Reserve, Winter'!M3*Scenarios!$B$7</f>
-        <v>33.729999999999997</v>
+        <v>25.297499999999999</v>
       </c>
       <c r="N3" s="2">
         <f>'[1]Secondary Reserve, Winter'!N3*Scenarios!$B$7</f>
-        <v>38.44</v>
+        <v>28.83</v>
       </c>
       <c r="O3" s="2">
         <f>'[1]Secondary Reserve, Winter'!O3*Scenarios!$B$7</f>
-        <v>28.68</v>
+        <v>21.509999999999998</v>
       </c>
       <c r="P3" s="2">
         <f>'[1]Secondary Reserve, Winter'!P3*Scenarios!$B$7</f>
-        <v>30.2</v>
+        <v>22.65</v>
       </c>
       <c r="Q3" s="2">
         <f>'[1]Secondary Reserve, Winter'!Q3*Scenarios!$B$7</f>
-        <v>27.12</v>
+        <v>20.34</v>
       </c>
       <c r="R3" s="2">
         <f>'[1]Secondary Reserve, Winter'!R3*Scenarios!$B$7</f>
-        <v>18.190000000000001</v>
+        <v>13.642500000000002</v>
       </c>
       <c r="S3" s="2">
         <f>'[1]Secondary Reserve, Winter'!S3*Scenarios!$B$7</f>
-        <v>22.68</v>
+        <v>17.009999999999998</v>
       </c>
       <c r="T3" s="2">
         <f>'[1]Secondary Reserve, Winter'!T3*Scenarios!$B$7</f>
-        <v>14.82</v>
+        <v>11.115</v>
       </c>
       <c r="U3" s="2">
         <f>'[1]Secondary Reserve, Winter'!U3*Scenarios!$B$7</f>
-        <v>13</v>
+        <v>9.75</v>
       </c>
       <c r="V3" s="2">
         <f>'[1]Secondary Reserve, Winter'!V3*Scenarios!$B$7</f>
-        <v>14.51</v>
+        <v>10.8825</v>
       </c>
       <c r="W3" s="2">
         <f>'[1]Secondary Reserve, Winter'!W3*Scenarios!$B$7</f>
-        <v>17.04</v>
+        <v>12.78</v>
       </c>
       <c r="X3" s="2">
         <f>'[1]Secondary Reserve, Winter'!X3*Scenarios!$B$7</f>
-        <v>18.21</v>
+        <v>13.657500000000001</v>
       </c>
       <c r="Y3" s="2">
         <f>'[1]Secondary Reserve, Winter'!Y3*Scenarios!$B$7</f>
-        <v>14</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3072,99 +3072,99 @@
       </c>
       <c r="B4" s="2">
         <f>'[1]Secondary Reserve, Winter'!B4*Scenarios!$B$7</f>
-        <v>16.43</v>
+        <v>27.930999999999997</v>
       </c>
       <c r="C4" s="2">
         <f>'[1]Secondary Reserve, Winter'!C4*Scenarios!$B$7</f>
-        <v>15.51</v>
+        <v>26.366999999999997</v>
       </c>
       <c r="D4" s="2">
         <f>'[1]Secondary Reserve, Winter'!D4*Scenarios!$B$7</f>
-        <v>16.440000000000001</v>
+        <v>27.948</v>
       </c>
       <c r="E4" s="2">
         <f>'[1]Secondary Reserve, Winter'!E4*Scenarios!$B$7</f>
-        <v>16.41</v>
+        <v>27.896999999999998</v>
       </c>
       <c r="F4" s="2">
         <f>'[1]Secondary Reserve, Winter'!F4*Scenarios!$B$7</f>
-        <v>16.920000000000002</v>
+        <v>28.764000000000003</v>
       </c>
       <c r="G4" s="2">
         <f>'[1]Secondary Reserve, Winter'!G4*Scenarios!$B$7</f>
-        <v>14.12</v>
+        <v>24.003999999999998</v>
       </c>
       <c r="H4" s="2">
         <f>'[1]Secondary Reserve, Winter'!H4*Scenarios!$B$7</f>
-        <v>12.35</v>
+        <v>20.994999999999997</v>
       </c>
       <c r="I4" s="2">
         <f>'[1]Secondary Reserve, Winter'!I4*Scenarios!$B$7</f>
-        <v>11.65</v>
+        <v>19.805</v>
       </c>
       <c r="J4" s="2">
         <f>'[1]Secondary Reserve, Winter'!J4*Scenarios!$B$7</f>
-        <v>10.45</v>
+        <v>17.764999999999997</v>
       </c>
       <c r="K4" s="2">
         <f>'[1]Secondary Reserve, Winter'!K4*Scenarios!$B$7</f>
-        <v>9.51</v>
+        <v>16.166999999999998</v>
       </c>
       <c r="L4" s="2">
         <f>'[1]Secondary Reserve, Winter'!L4*Scenarios!$B$7</f>
-        <v>7.8</v>
+        <v>13.26</v>
       </c>
       <c r="M4" s="2">
         <f>'[1]Secondary Reserve, Winter'!M4*Scenarios!$B$7</f>
-        <v>7.83</v>
+        <v>13.311</v>
       </c>
       <c r="N4" s="2">
         <f>'[1]Secondary Reserve, Winter'!N4*Scenarios!$B$7</f>
-        <v>8.5500000000000007</v>
+        <v>14.535</v>
       </c>
       <c r="O4" s="2">
         <f>'[1]Secondary Reserve, Winter'!O4*Scenarios!$B$7</f>
-        <v>8.5500000000000007</v>
+        <v>14.535</v>
       </c>
       <c r="P4" s="2">
         <f>'[1]Secondary Reserve, Winter'!P4*Scenarios!$B$7</f>
-        <v>9.5</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="Q4" s="2">
         <f>'[1]Secondary Reserve, Winter'!Q4*Scenarios!$B$7</f>
-        <v>7.45</v>
+        <v>12.664999999999999</v>
       </c>
       <c r="R4" s="2">
         <f>'[1]Secondary Reserve, Winter'!R4*Scenarios!$B$7</f>
-        <v>6.27</v>
+        <v>10.658999999999999</v>
       </c>
       <c r="S4" s="2">
         <f>'[1]Secondary Reserve, Winter'!S4*Scenarios!$B$7</f>
-        <v>6.98</v>
+        <v>11.866</v>
       </c>
       <c r="T4" s="2">
         <f>'[1]Secondary Reserve, Winter'!T4*Scenarios!$B$7</f>
-        <v>5.21</v>
+        <v>8.8569999999999993</v>
       </c>
       <c r="U4" s="2">
         <f>'[1]Secondary Reserve, Winter'!U4*Scenarios!$B$7</f>
-        <v>5.13</v>
+        <v>8.7210000000000001</v>
       </c>
       <c r="V4" s="2">
         <f>'[1]Secondary Reserve, Winter'!V4*Scenarios!$B$7</f>
-        <v>5.41</v>
+        <v>9.1969999999999992</v>
       </c>
       <c r="W4" s="2">
         <f>'[1]Secondary Reserve, Winter'!W4*Scenarios!$B$7</f>
-        <v>9.5</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="X4" s="2">
         <f>'[1]Secondary Reserve, Winter'!X4*Scenarios!$B$7</f>
-        <v>10.74</v>
+        <v>18.257999999999999</v>
       </c>
       <c r="Y4" s="2">
         <f>'[1]Secondary Reserve, Winter'!Y4*Scenarios!$B$7</f>
-        <v>10.74</v>
+        <v>18.257999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="D2" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!D2*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>24.97</v>
       </c>
       <c r="E2" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!E2*Scenarios!$B$9</f>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="F2" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!F2*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>25.97</v>
       </c>
       <c r="G2" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!G2*Scenarios!$B$9</f>
@@ -3891,99 +3891,99 @@
       </c>
       <c r="B3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!B3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>28.36</v>
       </c>
       <c r="C3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!C3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>28.36</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!D3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>27.234999999999999</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!E3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>28.86</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!F3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>28.86</v>
       </c>
       <c r="G3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!G3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>28.36</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!H3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>37.325000000000003</v>
       </c>
       <c r="I3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!I3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>30.75</v>
       </c>
       <c r="J3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!J3*Scenarios!$B$9</f>
-        <v>4.22</v>
+        <v>32.480000000000004</v>
       </c>
       <c r="K3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!K3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>34.879999999999995</v>
       </c>
       <c r="L3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!L3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.489999999999995</v>
       </c>
       <c r="M3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!M3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.489999999999995</v>
       </c>
       <c r="N3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!N3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.480000000000004</v>
       </c>
       <c r="O3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!O3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.5</v>
       </c>
       <c r="P3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!P3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.480000000000004</v>
       </c>
       <c r="Q3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!Q3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>32.480000000000004</v>
       </c>
       <c r="R3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!R3*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>34.885000000000005</v>
       </c>
       <c r="S3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!S3*Scenarios!$B$9</f>
-        <v>5.8</v>
+        <v>36.875</v>
       </c>
       <c r="T3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!T3*Scenarios!$B$9</f>
-        <v>5.9</v>
+        <v>36.875</v>
       </c>
       <c r="U3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!U3*Scenarios!$B$9</f>
-        <v>5.9</v>
+        <v>36.875</v>
       </c>
       <c r="V3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!V3*Scenarios!$B$9</f>
-        <v>6.1</v>
+        <v>36.875</v>
       </c>
       <c r="W3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!W3*Scenarios!$B$9</f>
-        <v>5.9</v>
+        <v>35.370000000000005</v>
       </c>
       <c r="X3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!X3*Scenarios!$B$9</f>
-        <v>5.6</v>
+        <v>30.75</v>
       </c>
       <c r="Y3" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!Y3*Scenarios!$B$9</f>
-        <v>36.6</v>
+        <v>30.75</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="B4" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!B4*Scenarios!$B$9</f>
-        <v>0</v>
+        <v>31.75</v>
       </c>
       <c r="C4" s="2">
         <f>'[1]Tertiary Reserve Down, Winter'!C4*Scenarios!$B$9</f>
@@ -4685,99 +4685,99 @@
       </c>
       <c r="B2" s="2">
         <f>'[1]Secondary Reserve, Summer'!B2*Scenarios!$B$7</f>
-        <v>7.99</v>
+        <v>10.26</v>
       </c>
       <c r="C2" s="2">
         <f>'[1]Secondary Reserve, Summer'!C2*Scenarios!$B$7</f>
-        <v>7.99</v>
+        <v>10.909500000000001</v>
       </c>
       <c r="D2" s="2">
         <f>'[1]Secondary Reserve, Summer'!D2*Scenarios!$B$7</f>
-        <v>7.99</v>
+        <v>10.084849999999999</v>
       </c>
       <c r="E2" s="2">
         <f>'[1]Secondary Reserve, Summer'!E2*Scenarios!$B$7</f>
-        <v>10.36</v>
+        <v>8.7750000000000004</v>
       </c>
       <c r="F2" s="2">
         <f>'[1]Secondary Reserve, Summer'!F2*Scenarios!$B$7</f>
-        <v>9.69</v>
+        <v>7.9588000000000001</v>
       </c>
       <c r="G2" s="2">
         <f>'[1]Secondary Reserve, Summer'!G2*Scenarios!$B$7</f>
-        <v>8.8800000000000008</v>
+        <v>6.3310499999999994</v>
       </c>
       <c r="H2" s="2">
         <f>'[1]Secondary Reserve, Summer'!H2*Scenarios!$B$7</f>
-        <v>8.09</v>
+        <v>5.706900000000001</v>
       </c>
       <c r="I2" s="2">
         <f>'[1]Secondary Reserve, Summer'!I2*Scenarios!$B$7</f>
-        <v>6.99</v>
+        <v>4.8929999999999998</v>
       </c>
       <c r="J2" s="2">
         <f>'[1]Secondary Reserve, Summer'!J2*Scenarios!$B$7</f>
-        <v>2.69</v>
+        <v>4.0228999999999999</v>
       </c>
       <c r="K2" s="2">
         <f>'[1]Secondary Reserve, Summer'!K2*Scenarios!$B$7</f>
-        <v>4.49</v>
+        <v>4.4879999999999995</v>
       </c>
       <c r="L2" s="2">
         <f>'[1]Secondary Reserve, Summer'!L2*Scenarios!$B$7</f>
-        <v>6.49</v>
+        <v>4.2223500000000005</v>
       </c>
       <c r="M2" s="2">
         <f>'[1]Secondary Reserve, Summer'!M2*Scenarios!$B$7</f>
-        <v>7.74</v>
+        <v>4.0441500000000001</v>
       </c>
       <c r="N2" s="2">
         <f>'[1]Secondary Reserve, Summer'!N2*Scenarios!$B$7</f>
-        <v>7.65</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="O2" s="2">
         <f>'[1]Secondary Reserve, Summer'!O2*Scenarios!$B$7</f>
-        <v>8.39</v>
+        <v>4.1912000000000003</v>
       </c>
       <c r="P2" s="2">
         <f>'[1]Secondary Reserve, Summer'!P2*Scenarios!$B$7</f>
-        <v>9.49</v>
+        <v>4.4894500000000006</v>
       </c>
       <c r="Q2" s="2">
         <f>'[1]Secondary Reserve, Summer'!Q2*Scenarios!$B$7</f>
-        <v>8.32</v>
+        <v>3.9945499999999998</v>
       </c>
       <c r="R2" s="2">
         <f>'[1]Secondary Reserve, Summer'!R2*Scenarios!$B$7</f>
-        <v>7.65</v>
+        <v>2.9760000000000004</v>
       </c>
       <c r="S2" s="2">
         <f>'[1]Secondary Reserve, Summer'!S2*Scenarios!$B$7</f>
-        <v>6.37</v>
+        <v>2.5608</v>
       </c>
       <c r="T2" s="2">
         <f>'[1]Secondary Reserve, Summer'!T2*Scenarios!$B$7</f>
-        <v>6.49</v>
+        <v>3.0141000000000004</v>
       </c>
       <c r="U2" s="2">
         <f>'[1]Secondary Reserve, Summer'!U2*Scenarios!$B$7</f>
-        <v>6.49</v>
+        <v>2.2196999999999996</v>
       </c>
       <c r="V2" s="2">
         <f>'[1]Secondary Reserve, Summer'!V2*Scenarios!$B$7</f>
-        <v>7.73</v>
+        <v>3.6414</v>
       </c>
       <c r="W2" s="2">
         <f>'[1]Secondary Reserve, Summer'!W2*Scenarios!$B$7</f>
-        <v>8.56</v>
+        <v>6.7825499999999996</v>
       </c>
       <c r="X2" s="2">
         <f>'[1]Secondary Reserve, Summer'!X2*Scenarios!$B$7</f>
-        <v>6.99</v>
+        <v>7.5711999999999993</v>
       </c>
       <c r="Y2" s="2">
         <f>'[1]Secondary Reserve, Summer'!Y2*Scenarios!$B$7</f>
-        <v>7.89</v>
+        <v>6.9015499999999994</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5158,99 +5158,99 @@
       </c>
       <c r="B2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!B2*Scenarios!$B$8</f>
-        <v>46.31</v>
+        <v>42.153333333333336</v>
       </c>
       <c r="C2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!C2*Scenarios!$B$8</f>
-        <v>46.31</v>
+        <v>42.486666666666672</v>
       </c>
       <c r="D2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!D2*Scenarios!$B$8</f>
-        <v>46.31</v>
+        <v>42.486666666666672</v>
       </c>
       <c r="E2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!E2*Scenarios!$B$8</f>
-        <v>64.64</v>
+        <v>51.303333333333335</v>
       </c>
       <c r="F2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!F2*Scenarios!$B$8</f>
-        <v>48.31</v>
+        <v>44.726666666666667</v>
       </c>
       <c r="G2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!G2*Scenarios!$B$8</f>
-        <v>42</v>
+        <v>53.636666666666677</v>
       </c>
       <c r="H2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!H2*Scenarios!$B$8</f>
-        <v>48.31</v>
+        <v>52.483333333333327</v>
       </c>
       <c r="I2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!I2*Scenarios!$B$8</f>
-        <v>42</v>
+        <v>40.266666666666673</v>
       </c>
       <c r="J2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!J2*Scenarios!$B$8</f>
-        <v>42</v>
+        <v>40.466666666666669</v>
       </c>
       <c r="K2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!K2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>59.133333333333333</v>
       </c>
       <c r="L2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!L2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.833333333333336</v>
       </c>
       <c r="M2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!M2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.833333333333336</v>
       </c>
       <c r="N2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!N2*Scenarios!$B$8</f>
-        <v>99</v>
+        <v>59.5</v>
       </c>
       <c r="O2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!O2*Scenarios!$B$8</f>
-        <v>99</v>
+        <v>59.5</v>
       </c>
       <c r="P2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!P2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>44.09</v>
       </c>
       <c r="Q2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!Q2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="R2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!R2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="S2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!S2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>41.06666666666667</v>
       </c>
       <c r="T2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!T2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.866666666666667</v>
       </c>
       <c r="U2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!U2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>44.09</v>
       </c>
       <c r="V2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!V2*Scenarios!$B$8</f>
-        <v>43</v>
+        <v>40.6</v>
       </c>
       <c r="W2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!W2*Scenarios!$B$8</f>
-        <v>48.31</v>
+        <v>45.860000000000007</v>
       </c>
       <c r="X2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!X2*Scenarios!$B$8</f>
-        <v>35.4</v>
+        <v>37.6</v>
       </c>
       <c r="Y2" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!Y2*Scenarios!$B$8</f>
-        <v>35.4</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5259,99 +5259,99 @@
       </c>
       <c r="B3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!B3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>36.216666666666669</v>
       </c>
       <c r="C3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!C3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>36.88333333333334</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!D3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>36.88333333333334</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!E3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>45.351666666666667</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!F3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>40.36333333333333</v>
       </c>
       <c r="G3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!G3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>61.338333333333338</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!H3*Scenarios!$B$8</f>
-        <v>40.1</v>
+        <v>60.76166666666667</v>
       </c>
       <c r="I3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!I3*Scenarios!$B$8</f>
-        <v>39.4</v>
+        <v>39.833333333333336</v>
       </c>
       <c r="J3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!J3*Scenarios!$B$8</f>
-        <v>39.4</v>
+        <v>40.233333333333334</v>
       </c>
       <c r="K3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!K3*Scenarios!$B$8</f>
-        <v>95</v>
+        <v>49.266666666666666</v>
       </c>
       <c r="L3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!L3*Scenarios!$B$8</f>
-        <v>40.1</v>
+        <v>40.116666666666667</v>
       </c>
       <c r="M3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!M3*Scenarios!$B$8</f>
-        <v>40.1</v>
+        <v>40.116666666666667</v>
       </c>
       <c r="N3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!N3*Scenarios!$B$8</f>
-        <v>40.1</v>
+        <v>49.45</v>
       </c>
       <c r="O3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!O3*Scenarios!$B$8</f>
-        <v>40.1</v>
+        <v>49.45</v>
       </c>
       <c r="P3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!P3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>41.745000000000005</v>
       </c>
       <c r="Q3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!Q3*Scenarios!$B$8</f>
-        <v>40</v>
+        <v>40.1</v>
       </c>
       <c r="R3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!R3*Scenarios!$B$8</f>
-        <v>39.4</v>
+        <v>40.400000000000006</v>
       </c>
       <c r="S3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!S3*Scenarios!$B$8</f>
-        <v>40</v>
+        <v>40.63333333333334</v>
       </c>
       <c r="T3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!T3*Scenarios!$B$8</f>
-        <v>39.4</v>
+        <v>40.533333333333331</v>
       </c>
       <c r="U3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!U3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>41.745000000000005</v>
       </c>
       <c r="V3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!V3*Scenarios!$B$8</f>
-        <v>39.4</v>
+        <v>40</v>
       </c>
       <c r="W3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!W3*Scenarios!$B$8</f>
-        <v>49.87</v>
+        <v>42.63</v>
       </c>
       <c r="X3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!X3*Scenarios!$B$8</f>
-        <v>37.4</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="Y3" s="2">
         <f>'[1]Tertiary Reserve Up, Summer'!Y3*Scenarios!$B$8</f>
-        <v>37.4</v>
+        <v>38.799999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -5706,99 +5706,99 @@
       </c>
       <c r="B3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!B3*Scenarios!$B$9</f>
-        <v>39.4</v>
+        <v>27.917499999999997</v>
       </c>
       <c r="C3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!C3*Scenarios!$B$9</f>
-        <v>39.4</v>
+        <v>27.917499999999997</v>
       </c>
       <c r="D3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!D3*Scenarios!$B$9</f>
-        <v>39.4</v>
+        <v>27.917499999999997</v>
       </c>
       <c r="E3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!E3*Scenarios!$B$9</f>
-        <v>39.4</v>
+        <v>27.917499999999997</v>
       </c>
       <c r="F3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!F3*Scenarios!$B$9</f>
-        <v>39.4</v>
+        <v>31.63</v>
       </c>
       <c r="G3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!G3*Scenarios!$B$9</f>
-        <v>7.06</v>
+        <v>23.537500000000001</v>
       </c>
       <c r="H3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!H3*Scenarios!$B$9</f>
-        <v>29.97</v>
+        <v>29.28</v>
       </c>
       <c r="I3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!I3*Scenarios!$B$9</f>
-        <v>20.55</v>
+        <v>26.9175</v>
       </c>
       <c r="J3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!J3*Scenarios!$B$9</f>
-        <v>20.55</v>
+        <v>26.9175</v>
       </c>
       <c r="K3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!K3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.950000000000003</v>
       </c>
       <c r="L3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!L3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>33.162500000000001</v>
       </c>
       <c r="M3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!M3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.935000000000002</v>
       </c>
       <c r="N3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!N3*Scenarios!$B$9</f>
-        <v>29.97</v>
+        <v>29.265000000000001</v>
       </c>
       <c r="O3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!O3*Scenarios!$B$9</f>
-        <v>29.97</v>
+        <v>29.265000000000001</v>
       </c>
       <c r="P3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!P3*Scenarios!$B$9</f>
-        <v>29.97</v>
+        <v>31.4925</v>
       </c>
       <c r="Q3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!Q3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.92</v>
       </c>
       <c r="R3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!R3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>33.162500000000001</v>
       </c>
       <c r="S3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!S3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.92</v>
       </c>
       <c r="T3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!T3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.92</v>
       </c>
       <c r="U3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!U3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.92</v>
       </c>
       <c r="V3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!V3*Scenarios!$B$9</f>
-        <v>36.65</v>
+        <v>30.92</v>
       </c>
       <c r="W3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!W3*Scenarios!$B$9</f>
-        <v>29.97</v>
+        <v>29.25</v>
       </c>
       <c r="X3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!X3*Scenarios!$B$9</f>
-        <v>26.19</v>
+        <v>28.305</v>
       </c>
       <c r="Y3" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!Y3*Scenarios!$B$9</f>
-        <v>26.19</v>
+        <v>27.532499999999999</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -5807,99 +5807,99 @@
       </c>
       <c r="B4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!B4*Scenarios!$B$9</f>
-        <v>2.2200000000000002</v>
+        <v>31.744999999999997</v>
       </c>
       <c r="C4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!C4*Scenarios!$B$9</f>
-        <v>2.2000000000000002</v>
+        <v>31.744999999999997</v>
       </c>
       <c r="D4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!D4*Scenarios!$B$9</f>
-        <v>2.2200000000000002</v>
+        <v>31.744999999999997</v>
       </c>
       <c r="E4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!E4*Scenarios!$B$9</f>
-        <v>2.2200000000000002</v>
+        <v>31.744999999999997</v>
       </c>
       <c r="F4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!F4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>34.22</v>
       </c>
       <c r="G4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!G4*Scenarios!$B$9</f>
-        <v>37.520000000000003</v>
+        <v>18.045000000000002</v>
       </c>
       <c r="H4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!H4*Scenarios!$B$9</f>
-        <v>37.520000000000003</v>
+        <v>29.509999999999998</v>
       </c>
       <c r="I4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!I4*Scenarios!$B$9</f>
-        <v>20.02</v>
+        <v>24.795000000000002</v>
       </c>
       <c r="J4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!J4*Scenarios!$B$9</f>
-        <v>26</v>
+        <v>24.795000000000002</v>
       </c>
       <c r="K4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!K4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.85</v>
       </c>
       <c r="L4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!L4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>34.325000000000003</v>
       </c>
       <c r="M4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!M4*Scenarios!$B$9</f>
-        <v>37.9</v>
+        <v>32.840000000000003</v>
       </c>
       <c r="N4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!N4*Scenarios!$B$9</f>
-        <v>37.9</v>
+        <v>29.5</v>
       </c>
       <c r="O4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!O4*Scenarios!$B$9</f>
-        <v>37.9</v>
+        <v>29.5</v>
       </c>
       <c r="P4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!P4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>30.984999999999999</v>
       </c>
       <c r="Q4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!Q4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.83</v>
       </c>
       <c r="R4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!R4*Scenarios!$B$9</f>
-        <v>25.67</v>
+        <v>34.325000000000003</v>
       </c>
       <c r="S4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!S4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.83</v>
       </c>
       <c r="T4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!T4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.83</v>
       </c>
       <c r="U4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!U4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.83</v>
       </c>
       <c r="V4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!V4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>32.83</v>
       </c>
       <c r="W4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!W4*Scenarios!$B$9</f>
-        <v>37.51</v>
+        <v>29.490000000000002</v>
       </c>
       <c r="X4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!X4*Scenarios!$B$9</f>
-        <v>30.19</v>
+        <v>27.6</v>
       </c>
       <c r="Y4" s="2">
         <f>'[1]Tertiary Reserve Down, Summer'!Y4*Scenarios!$B$9</f>
-        <v>30.19</v>
+        <v>27.085000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>